<commit_message>
added nutrition (up to salt intake)
</commit_message>
<xml_diff>
--- a/input/STEPS_Instrument_V3_2_1_V3.xlsx
+++ b/input/STEPS_Instrument_V3_2_1_V3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{269CBCFD-9F07-4661-8C8E-7F8A5A0B7AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1545" windowWidth="20910" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6555" yWindow="390" windowWidth="20910" windowHeight="13845" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -5497,11 +5497,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T316"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N177" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="N94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N30" sqref="N30"/>
+      <selection pane="bottomRight" activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15113,9 +15113,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F394"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D133" sqref="D133:D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>